<commit_message>
Update multiple features: Password reveal, Notification repository, Dosen updates and SQL structure
This update brings several changes. The password reveal functionality now targets any password and text field within the parent element. New Notification Repository has been added for handling notifications effectively. The Dosen feature has been enhanced with better Prodi sync and addition of new Fakultas field. Alongside, SQL structure has also observed some additional entities in schema as well as data.
</commit_message>
<xml_diff>
--- a/templates/dosen_template.xlsx
+++ b/templates/dosen_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericanthony/Projects/nodejs-fullstack/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE04AAF7-763E-6A42-BC1F-69002F026773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0461A2-3BF9-B948-AF1F-0B8FB3DAD8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{71D497EA-3604-9444-B02E-D894D6915CD7}"/>
+    <workbookView xWindow="4880" yWindow="500" windowWidth="46320" windowHeight="26380" xr2:uid="{71D497EA-3604-9444-B02E-D894D6915CD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
   <si>
     <t>Dosen 1</t>
   </si>
@@ -291,6 +291,21 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>fakultas</t>
+  </si>
+  <si>
+    <t>Pendidikan Profesi Psikologi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Profesi Akuntan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Sistem Informasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Teknik Informatika</t>
   </si>
 </sst>
 </file>
@@ -679,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70C0AF1-D524-C648-87F6-9FE27824C683}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +709,7 @@
     <col min="5" max="5" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -708,10 +723,13 @@
         <v>84</v>
       </c>
       <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -725,10 +743,13 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -742,10 +763,13 @@
         <v>49</v>
       </c>
       <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -759,10 +783,13 @@
         <v>50</v>
       </c>
       <c r="E4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -776,10 +803,13 @@
         <v>51</v>
       </c>
       <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -793,10 +823,13 @@
         <v>52</v>
       </c>
       <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -810,10 +843,13 @@
         <v>53</v>
       </c>
       <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -827,10 +863,13 @@
         <v>54</v>
       </c>
       <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -844,10 +883,13 @@
         <v>55</v>
       </c>
       <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -861,10 +903,13 @@
         <v>56</v>
       </c>
       <c r="E10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -878,10 +923,13 @@
         <v>57</v>
       </c>
       <c r="E11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -895,10 +943,13 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -912,10 +963,13 @@
         <v>59</v>
       </c>
       <c r="E13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -929,10 +983,13 @@
         <v>60</v>
       </c>
       <c r="E14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -946,10 +1003,13 @@
         <v>61</v>
       </c>
       <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -963,10 +1023,13 @@
         <v>62</v>
       </c>
       <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -980,6 +1043,9 @@
         <v>63</v>
       </c>
       <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update fakultas field to prodi
The term 'fakultas' has been replaced with 'prodi' throughout the system, in both labels and handling of data. This includes changes in the database query to restrict the selection of degrees to 'Teknik Informatika' and 'Sistem Informasi'.
</commit_message>
<xml_diff>
--- a/templates/dosen_template.xlsx
+++ b/templates/dosen_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericanthony/Projects/nodejs-fullstack/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0461A2-3BF9-B948-AF1F-0B8FB3DAD8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD7900A-241A-3341-9183-D17E0E16B6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="500" windowWidth="46320" windowHeight="26380" xr2:uid="{71D497EA-3604-9444-B02E-D894D6915CD7}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17580" xr2:uid="{71D497EA-3604-9444-B02E-D894D6915CD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,19 +293,19 @@
     <t>email</t>
   </si>
   <si>
-    <t>fakultas</t>
-  </si>
-  <si>
     <t>Pendidikan Profesi Psikologi</t>
   </si>
   <si>
-    <t xml:space="preserve">	Profesi Akuntan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Sistem Informasi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Teknik Informatika</t>
+    <t>prodi</t>
+  </si>
+  <si>
+    <t>Teknik Informatika</t>
+  </si>
+  <si>
+    <t>Profesi Akuntan</t>
+  </si>
+  <si>
+    <t>Sistem Informasi</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,7 +723,7 @@
         <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
         <v>82</v>
@@ -743,7 +743,7 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>64</v>
@@ -763,7 +763,7 @@
         <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
@@ -783,7 +783,7 @@
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -803,7 +803,7 @@
         <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
         <v>67</v>
@@ -823,7 +823,7 @@
         <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
         <v>68</v>
@@ -843,7 +843,7 @@
         <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
         <v>69</v>
@@ -863,7 +863,7 @@
         <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
         <v>70</v>
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
         <v>71</v>
@@ -903,7 +903,7 @@
         <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
         <v>72</v>
@@ -923,7 +923,7 @@
         <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
         <v>73</v>
@@ -943,7 +943,7 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
         <v>74</v>
@@ -963,7 +963,7 @@
         <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
         <v>75</v>
@@ -983,7 +983,7 @@
         <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
         <v>76</v>
@@ -1003,7 +1003,7 @@
         <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
         <v>77</v>
@@ -1023,7 +1023,7 @@
         <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
         <v>78</v>
@@ -1043,7 +1043,7 @@
         <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F17" t="s">
         <v>79</v>

</xml_diff>